<commit_message>
modify team 4 name
</commit_message>
<xml_diff>
--- a/2024_OSS_Project_Peer_Review.xlsx
+++ b/2024_OSS_Project_Peer_Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\[강의]\광운대학교 강의\2024-2 오픈소스소프트웨어설계및실습\프로젝트\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shin\Dropbox\[강의]\광운대학교 강의\2024-2 오픈소스소프트웨어설계및실습\프로젝트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2109F6A0-9FD8-4D5B-B159-7F0C9928E315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C90FDA-EB9D-4105-81B8-464F84C127F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="2475" windowWidth="27165" windowHeight="15885" xr2:uid="{5F4F1681-583B-4F87-B592-A8DAFB1E07BC}"/>
+    <workbookView xWindow="830" yWindow="-110" windowWidth="37680" windowHeight="21820" xr2:uid="{5F4F1681-583B-4F87-B592-A8DAFB1E07BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,10 +65,6 @@
   </si>
   <si>
     <t>KW-MatchRoomie</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주니어 광운</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -262,6 +258,10 @@
   <si>
     <t>※ Note: If you include your own team in the evaluation, if there are ties in the Level of Completion rankings, or if you fail to provide even a brief rationale, points will be deducted from your personal score. Please be sure to complete the form with care.
 ※ 주의: 자기 조도 포함하여 평가를 하거나, Level of Completion 의 순위가 중복되거나, Rationale을 간단하게라도 작성하지 않은 경우는 개인 점수에서 감점이 될 것이니, 꼭 주의해서 작성 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팡팡랜드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -728,74 +728,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D54108-E716-42BF-9494-7C0647B99379}">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="38.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="3" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="7" spans="2:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="11" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
@@ -809,10 +809,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -834,7 +834,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="1">
         <v>3</v>
       </c>
@@ -845,130 +845,130 @@
       <c r="E14" s="1"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="1">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1">
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1">
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1">
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="27" spans="2:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="81" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>

</xml_diff>